<commit_message>
Changed the if condition in AndroidCaller.java file
</commit_message>
<xml_diff>
--- a/ExcelFiles/ExcelInput.xlsx
+++ b/ExcelFiles/ExcelInput.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10614"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vinaygopinath/IdeaProjects/ECommerceAppAutomation/ExcelFiles/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vinaygopinath/ECommerceAppAutomation/ExcelFiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{940BF4A1-EEBE-8447-8110-07B71517EE4F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3289F843-A8BE-A948-A4D0-E0B305655B76}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16540" xr2:uid="{0F47F944-E0BE-DA4A-8FE8-623DD97EEEC5}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="15">
   <si>
     <t>SL No</t>
   </si>
@@ -75,6 +75,9 @@
   </si>
   <si>
     <t>PASS</t>
+  </si>
+  <si>
+    <t>FAIL</t>
   </si>
 </sst>
 </file>
@@ -441,7 +444,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="D2" sqref="D2:D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -503,7 +506,7 @@
         <v>5</v>
       </c>
       <c r="D4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -517,7 +520,7 @@
         <v>6</v>
       </c>
       <c r="D5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
paramatrized the class<?> and Constructor<?> in AndfordCaller.java
</commit_message>
<xml_diff>
--- a/ExcelFiles/ExcelInput.xlsx
+++ b/ExcelFiles/ExcelInput.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vinaygopinath/ECommerceAppAutomation/ExcelFiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3289F843-A8BE-A948-A4D0-E0B305655B76}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01ECBA4B-F886-1042-904E-95780FE9A13A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16540" xr2:uid="{0F47F944-E0BE-DA4A-8FE8-623DD97EEEC5}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="14">
   <si>
     <t>SL No</t>
   </si>
@@ -71,13 +71,10 @@
     <t>This test case will test the toast Message</t>
   </si>
   <si>
-    <t>NO RUN</t>
+    <t>FAIL</t>
   </si>
   <si>
     <t>PASS</t>
-  </si>
-  <si>
-    <t>FAIL</t>
   </si>
 </sst>
 </file>
@@ -506,7 +503,7 @@
         <v>5</v>
       </c>
       <c r="D4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -520,7 +517,7 @@
         <v>6</v>
       </c>
       <c r="D5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added functionalities related to mobile browser automation
</commit_message>
<xml_diff>
--- a/ExcelFiles/ExcelInput.xlsx
+++ b/ExcelFiles/ExcelInput.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vinaygopinath/ECommerceAppAutomation/ExcelFiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01ECBA4B-F886-1042-904E-95780FE9A13A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{671B004F-C7DF-0B40-B831-350C7C8500DB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16540" xr2:uid="{0F47F944-E0BE-DA4A-8FE8-623DD97EEEC5}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="14">
   <si>
     <t>SL No</t>
   </si>
@@ -441,7 +441,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D5"/>
+      <selection activeCell="D5" sqref="D2:D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
code structure changed and updated the chrome driver.
</commit_message>
<xml_diff>
--- a/ExcelFiles/ExcelInput.xlsx
+++ b/ExcelFiles/ExcelInput.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vinaygopinath/ECommerceAppAutomation/ExcelFiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{671B004F-C7DF-0B40-B831-350C7C8500DB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5A2850E-DEAE-A449-BF7F-08601A874078}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16540" xr2:uid="{0F47F944-E0BE-DA4A-8FE8-623DD97EEEC5}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="14">
   <si>
     <t>SL No</t>
   </si>
@@ -441,7 +441,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D2:D5"/>
+      <selection activeCell="D2" sqref="D2:D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
no code changes. Just cosmetic changes
</commit_message>
<xml_diff>
--- a/ExcelFiles/ExcelInput.xlsx
+++ b/ExcelFiles/ExcelInput.xlsx
@@ -3,12 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vinaygopinath/ECommerceAppAutomation/ExcelFiles/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vinaygopinath/IdeaProjects/ECommerceAppAutomation/ExcelFiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5A2850E-DEAE-A449-BF7F-08601A874078}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A15405E-4399-EA4F-BE43-D514749D6682}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16540" xr2:uid="{0F47F944-E0BE-DA4A-8FE8-623DD97EEEC5}"/>
   </bookViews>
@@ -17,7 +17,7 @@
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
   <si>
     <t>SL No</t>
   </si>
@@ -81,7 +81,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -441,13 +440,13 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D4"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="44.33203125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="25.1640625" collapsed="true"/>
+    <col min="2" max="2" width="44.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="25.1640625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="1" customFormat="1" ht="28" customHeight="1" x14ac:dyDescent="0.2">
@@ -475,7 +474,7 @@
         <v>3</v>
       </c>
       <c r="D2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
changes in Appium Capabilities
</commit_message>
<xml_diff>
--- a/ExcelFiles/ExcelInput.xlsx
+++ b/ExcelFiles/ExcelInput.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vinaygopinath/IdeaProjects/ECommerceAppAutomation/ExcelFiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A15405E-4399-EA4F-BE43-D514749D6682}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28882AB0-538E-B540-8043-36F63A190D9C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16540" xr2:uid="{0F47F944-E0BE-DA4A-8FE8-623DD97EEEC5}"/>
+    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16540" xr2:uid="{0F47F944-E0BE-DA4A-8FE8-623DD97EEEC5}"/>
   </bookViews>
   <sheets>
     <sheet name="UserDataForm" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="15">
   <si>
     <t>SL No</t>
   </si>
@@ -71,16 +71,20 @@
     <t>This test case will test the toast Message</t>
   </si>
   <si>
+    <t>FAIl</t>
+  </si>
+  <si>
+    <t>PASS</t>
+  </si>
+  <si>
     <t>FAIL</t>
-  </si>
-  <si>
-    <t>PASS</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -440,13 +444,13 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="D2" sqref="D2:D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="44.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="25.1640625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="44.33203125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="25.1640625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="1" customFormat="1" ht="28" customHeight="1" x14ac:dyDescent="0.2">
@@ -474,7 +478,7 @@
         <v>3</v>
       </c>
       <c r="D2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -516,7 +520,7 @@
         <v>6</v>
       </c>
       <c r="D5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modifications with new version of chrome driver for windows 11
</commit_message>
<xml_diff>
--- a/ExcelFiles/ExcelInput.xlsx
+++ b/ExcelFiles/ExcelInput.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vinaygopinath/IdeaProjects/ECommerceAppAutomation/ExcelFiles/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nichiuser\IdeaProjects\ECommerceAppAutomation\ExcelFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28882AB0-538E-B540-8043-36F63A190D9C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1CD5146-F383-4D01-BC91-112CADE7A8BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16540" xr2:uid="{0F47F944-E0BE-DA4A-8FE8-623DD97EEEC5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{0F47F944-E0BE-DA4A-8FE8-623DD97EEEC5}"/>
   </bookViews>
   <sheets>
     <sheet name="UserDataForm" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="15">
   <si>
     <t>SL No</t>
   </si>
@@ -71,7 +71,7 @@
     <t>This test case will test the toast Message</t>
   </si>
   <si>
-    <t>FAIl</t>
+    <t>No RUN</t>
   </si>
   <si>
     <t>PASS</t>
@@ -444,16 +444,16 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D5"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="44.33203125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="25.1640625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="44.375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="25.125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" s="1" customFormat="1" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -467,7 +467,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -481,7 +481,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -495,7 +495,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -509,7 +509,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>

</xml_diff>